<commit_message>
poriadok odstranenie bakalarky z hlavneho adresara a ponechanie v bakalarka-pdf
</commit_message>
<xml_diff>
--- a/resources/Hardware parts/prepocet vzorkovania ADC.xlsx
+++ b/resources/Hardware parts/prepocet vzorkovania ADC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VUT\bakalarka\resources\Hardware parts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{907ECD42-8E43-47BA-96B4-4AA1721A086B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{204FC320-A9BA-4A0C-AA67-3EC40E6A35C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="-15870" windowWidth="25440" windowHeight="15390" xr2:uid="{42EF5C74-19FC-45CF-975D-7BDBA201D871}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{42EF5C74-19FC-45CF-975D-7BDBA201D871}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="20">
   <si>
     <t>cm</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>x viac vzoriek dostanem</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -443,13 +446,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70C17714-4430-4014-9B78-33A6B40DA242}">
-  <dimension ref="A3:P32"/>
+  <dimension ref="A3:P33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+      <selection activeCell="O16" sqref="O16:U19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="15" max="15" width="11.5546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -683,6 +689,11 @@
         <v>18</v>
       </c>
     </row>
+    <row r="33" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F33" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>